<commit_message>
The actual final update
</commit_message>
<xml_diff>
--- a/MedicalRecords.xlsx
+++ b/MedicalRecords.xlsx
@@ -28,6 +28,14 @@
     <x:sheet name="Record  20210127 170407" sheetId="18" r:id="rId18"/>
     <x:sheet name="Record  20210127 171903" sheetId="19" r:id="rId19"/>
     <x:sheet name="Record  20210127 181035" sheetId="20" r:id="rId20"/>
+    <x:sheet name="Record  20210131 150830" sheetId="21" r:id="rId21"/>
+    <x:sheet name="Record  20210131 152811" sheetId="22" r:id="rId22"/>
+    <x:sheet name="Record  20210131 153656" sheetId="23" r:id="rId23"/>
+    <x:sheet name="Record  20210131 153757" sheetId="24" r:id="rId24"/>
+    <x:sheet name="Record  20210131 153843" sheetId="25" r:id="rId25"/>
+    <x:sheet name="Record  20210131 184433" sheetId="26" r:id="rId26"/>
+    <x:sheet name="Record  20210131 185329" sheetId="27" r:id="rId27"/>
+    <x:sheet name="Record  20210131 193251" sheetId="28" r:id="rId28"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="0"/>
@@ -1798,6 +1806,4758 @@
 </x:worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:K17"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:11">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:11">
+      <x:c r="A2" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E2" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G2" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I2" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="J2" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K2" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
+      <x:c r="A3" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I3" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J3" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K3" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:11">
+      <x:c r="A4" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G4" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I4" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J4" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K4" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11">
+      <x:c r="A5" s="2" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D5" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I5" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J5" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K5" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:11">
+      <x:c r="A6" s="2" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B6" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E6" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I6" s="2" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J6" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K6" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:11">
+      <x:c r="A7" s="2" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B7" s="2" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E7" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H7" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I7" s="2" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="J7" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K7" s="2" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:11">
+      <x:c r="A8" s="2" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C8" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G8" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I8" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J8" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K8" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:11">
+      <x:c r="A9" s="2" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B9" s="2" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="C9" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E9" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I9" s="2" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="J9" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K9" s="2" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:11">
+      <x:c r="A10" s="2" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B10" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C10" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D10" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E10" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I10" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J10" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K10" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:11">
+      <x:c r="A11" s="2" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B11" s="2" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C11" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E11" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I11" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J11" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K11" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:11">
+      <x:c r="A12" s="2" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B12" s="2" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C12" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F12" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I12" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J12" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K12" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:11">
+      <x:c r="A13" s="2" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B13" s="2" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C13" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I13" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J13" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K13" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:11">
+      <x:c r="A14" s="2" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B14" s="2" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C14" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I14" s="2" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="J14" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K14" s="2" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:11">
+      <x:c r="A15" s="2" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B15" s="2" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C15" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F15" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H15" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I15" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J15" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K15" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:11">
+      <x:c r="A16" s="2" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B16" s="2" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C16" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D16" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I16" s="2" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="J16" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K16" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:11">
+      <x:c r="A17" s="2" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B17" s="2" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C17" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E17" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G17" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I17" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J17" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K17" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:K17"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:11">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:11">
+      <x:c r="A2" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E2" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G2" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I2" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="J2" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K2" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
+      <x:c r="A3" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I3" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J3" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K3" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:11">
+      <x:c r="A4" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G4" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I4" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J4" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K4" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11">
+      <x:c r="A5" s="2" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D5" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I5" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J5" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K5" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:11">
+      <x:c r="A6" s="2" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B6" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E6" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I6" s="2" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J6" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K6" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:11">
+      <x:c r="A7" s="2" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B7" s="2" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E7" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H7" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I7" s="2" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="J7" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K7" s="2" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:11">
+      <x:c r="A8" s="2" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C8" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G8" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I8" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J8" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K8" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:11">
+      <x:c r="A9" s="2" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B9" s="2" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="C9" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E9" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I9" s="2" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="J9" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K9" s="2" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:11">
+      <x:c r="A10" s="2" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B10" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C10" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D10" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E10" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I10" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J10" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K10" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:11">
+      <x:c r="A11" s="2" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B11" s="2" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C11" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E11" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I11" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J11" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K11" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:11">
+      <x:c r="A12" s="2" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B12" s="2" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C12" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F12" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I12" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J12" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K12" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:11">
+      <x:c r="A13" s="2" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B13" s="2" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C13" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I13" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J13" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K13" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:11">
+      <x:c r="A14" s="2" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B14" s="2" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C14" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I14" s="2" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="J14" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K14" s="2" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:11">
+      <x:c r="A15" s="2" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B15" s="2" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C15" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F15" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H15" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I15" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J15" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K15" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:11">
+      <x:c r="A16" s="2" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B16" s="2" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C16" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D16" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I16" s="2" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="J16" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K16" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:11">
+      <x:c r="A17" s="2" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B17" s="2" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C17" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E17" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G17" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I17" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J17" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K17" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:K17"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:11">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:11">
+      <x:c r="A2" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E2" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G2" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I2" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="J2" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K2" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
+      <x:c r="A3" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I3" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J3" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K3" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:11">
+      <x:c r="A4" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G4" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I4" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J4" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K4" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11">
+      <x:c r="A5" s="2" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D5" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I5" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J5" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K5" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:11">
+      <x:c r="A6" s="2" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B6" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E6" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I6" s="2" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J6" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K6" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:11">
+      <x:c r="A7" s="2" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B7" s="2" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E7" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H7" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I7" s="2" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="J7" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K7" s="2" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:11">
+      <x:c r="A8" s="2" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C8" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G8" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I8" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J8" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K8" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:11">
+      <x:c r="A9" s="2" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B9" s="2" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="C9" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E9" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I9" s="2" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="J9" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K9" s="2" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:11">
+      <x:c r="A10" s="2" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B10" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C10" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D10" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E10" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I10" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J10" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K10" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:11">
+      <x:c r="A11" s="2" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B11" s="2" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C11" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E11" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I11" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J11" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K11" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:11">
+      <x:c r="A12" s="2" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B12" s="2" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C12" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F12" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I12" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J12" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K12" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:11">
+      <x:c r="A13" s="2" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B13" s="2" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C13" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I13" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J13" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K13" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:11">
+      <x:c r="A14" s="2" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B14" s="2" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C14" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I14" s="2" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="J14" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K14" s="2" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:11">
+      <x:c r="A15" s="2" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B15" s="2" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C15" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F15" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H15" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I15" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J15" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K15" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:11">
+      <x:c r="A16" s="2" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B16" s="2" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C16" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D16" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I16" s="2" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="J16" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K16" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:11">
+      <x:c r="A17" s="2" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B17" s="2" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C17" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E17" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G17" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I17" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J17" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K17" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:K17"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:11">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:11">
+      <x:c r="A2" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E2" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G2" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I2" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="J2" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K2" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
+      <x:c r="A3" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I3" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J3" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K3" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:11">
+      <x:c r="A4" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G4" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I4" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J4" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K4" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11">
+      <x:c r="A5" s="2" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D5" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I5" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J5" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K5" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:11">
+      <x:c r="A6" s="2" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B6" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E6" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I6" s="2" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J6" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K6" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:11">
+      <x:c r="A7" s="2" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B7" s="2" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E7" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H7" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I7" s="2" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="J7" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K7" s="2" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:11">
+      <x:c r="A8" s="2" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C8" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G8" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I8" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J8" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K8" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:11">
+      <x:c r="A9" s="2" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B9" s="2" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="C9" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E9" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I9" s="2" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="J9" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K9" s="2" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:11">
+      <x:c r="A10" s="2" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B10" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C10" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D10" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E10" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I10" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J10" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K10" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:11">
+      <x:c r="A11" s="2" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B11" s="2" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C11" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E11" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I11" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J11" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K11" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:11">
+      <x:c r="A12" s="2" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B12" s="2" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C12" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F12" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I12" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J12" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K12" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:11">
+      <x:c r="A13" s="2" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B13" s="2" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C13" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I13" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J13" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K13" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:11">
+      <x:c r="A14" s="2" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B14" s="2" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C14" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I14" s="2" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="J14" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K14" s="2" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:11">
+      <x:c r="A15" s="2" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B15" s="2" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C15" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F15" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H15" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I15" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J15" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K15" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:11">
+      <x:c r="A16" s="2" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B16" s="2" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C16" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D16" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I16" s="2" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="J16" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K16" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:11">
+      <x:c r="A17" s="2" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B17" s="2" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C17" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E17" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G17" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I17" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J17" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K17" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:K17"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:11">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:11">
+      <x:c r="A2" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E2" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G2" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I2" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="J2" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K2" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
+      <x:c r="A3" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I3" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J3" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K3" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:11">
+      <x:c r="A4" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G4" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I4" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J4" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K4" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11">
+      <x:c r="A5" s="2" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D5" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I5" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J5" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K5" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:11">
+      <x:c r="A6" s="2" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B6" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E6" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I6" s="2" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J6" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K6" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:11">
+      <x:c r="A7" s="2" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B7" s="2" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E7" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H7" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I7" s="2" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="J7" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K7" s="2" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:11">
+      <x:c r="A8" s="2" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C8" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G8" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I8" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J8" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K8" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:11">
+      <x:c r="A9" s="2" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B9" s="2" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="C9" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E9" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I9" s="2" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="J9" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K9" s="2" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:11">
+      <x:c r="A10" s="2" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B10" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C10" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D10" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E10" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I10" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J10" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K10" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:11">
+      <x:c r="A11" s="2" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B11" s="2" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C11" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E11" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I11" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J11" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K11" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:11">
+      <x:c r="A12" s="2" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B12" s="2" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C12" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F12" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I12" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J12" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K12" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:11">
+      <x:c r="A13" s="2" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B13" s="2" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C13" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I13" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J13" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K13" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:11">
+      <x:c r="A14" s="2" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B14" s="2" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C14" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I14" s="2" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="J14" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K14" s="2" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:11">
+      <x:c r="A15" s="2" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B15" s="2" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C15" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F15" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H15" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I15" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J15" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K15" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:11">
+      <x:c r="A16" s="2" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B16" s="2" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C16" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D16" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I16" s="2" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="J16" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K16" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:11">
+      <x:c r="A17" s="2" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B17" s="2" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C17" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E17" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G17" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I17" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J17" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K17" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:K17"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:11">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:11">
+      <x:c r="A2" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E2" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G2" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I2" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="J2" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K2" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
+      <x:c r="A3" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I3" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J3" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K3" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:11">
+      <x:c r="A4" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G4" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I4" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J4" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K4" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11">
+      <x:c r="A5" s="2" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D5" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I5" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J5" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K5" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:11">
+      <x:c r="A6" s="2" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B6" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E6" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I6" s="2" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J6" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K6" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:11">
+      <x:c r="A7" s="2" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B7" s="2" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E7" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H7" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I7" s="2" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="J7" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K7" s="2" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:11">
+      <x:c r="A8" s="2" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C8" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G8" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I8" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J8" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K8" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:11">
+      <x:c r="A9" s="2" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B9" s="2" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="C9" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E9" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I9" s="2" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="J9" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K9" s="2" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:11">
+      <x:c r="A10" s="2" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B10" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C10" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D10" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E10" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I10" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J10" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K10" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:11">
+      <x:c r="A11" s="2" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B11" s="2" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C11" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E11" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I11" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J11" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K11" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:11">
+      <x:c r="A12" s="2" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B12" s="2" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C12" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F12" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I12" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J12" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K12" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:11">
+      <x:c r="A13" s="2" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B13" s="2" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C13" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I13" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J13" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K13" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:11">
+      <x:c r="A14" s="2" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B14" s="2" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C14" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I14" s="2" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="J14" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K14" s="2" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:11">
+      <x:c r="A15" s="2" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B15" s="2" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C15" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F15" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H15" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I15" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J15" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K15" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:11">
+      <x:c r="A16" s="2" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B16" s="2" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C16" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D16" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I16" s="2" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="J16" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K16" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:11">
+      <x:c r="A17" s="2" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B17" s="2" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C17" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E17" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G17" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I17" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J17" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K17" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:K17"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:11">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:11">
+      <x:c r="A2" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E2" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G2" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I2" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="J2" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K2" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
+      <x:c r="A3" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I3" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J3" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K3" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:11">
+      <x:c r="A4" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G4" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I4" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J4" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K4" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11">
+      <x:c r="A5" s="2" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D5" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I5" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J5" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K5" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:11">
+      <x:c r="A6" s="2" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B6" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E6" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I6" s="2" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J6" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K6" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:11">
+      <x:c r="A7" s="2" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B7" s="2" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E7" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H7" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I7" s="2" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="J7" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K7" s="2" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:11">
+      <x:c r="A8" s="2" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C8" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G8" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I8" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J8" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K8" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:11">
+      <x:c r="A9" s="2" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B9" s="2" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="C9" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E9" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I9" s="2" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="J9" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K9" s="2" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:11">
+      <x:c r="A10" s="2" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B10" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C10" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D10" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E10" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I10" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J10" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K10" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:11">
+      <x:c r="A11" s="2" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B11" s="2" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C11" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E11" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I11" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J11" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K11" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:11">
+      <x:c r="A12" s="2" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B12" s="2" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C12" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F12" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I12" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J12" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K12" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:11">
+      <x:c r="A13" s="2" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B13" s="2" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C13" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I13" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J13" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K13" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:11">
+      <x:c r="A14" s="2" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B14" s="2" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C14" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I14" s="2" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="J14" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K14" s="2" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:11">
+      <x:c r="A15" s="2" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B15" s="2" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C15" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F15" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H15" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I15" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J15" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K15" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:11">
+      <x:c r="A16" s="2" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B16" s="2" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C16" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D16" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I16" s="2" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="J16" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K16" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:11">
+      <x:c r="A17" s="2" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B17" s="2" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C17" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E17" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G17" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I17" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J17" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K17" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:K17"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:11">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:11">
+      <x:c r="A2" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E2" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G2" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I2" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="J2" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K2" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
+      <x:c r="A3" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I3" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J3" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K3" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:11">
+      <x:c r="A4" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G4" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H4" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I4" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J4" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K4" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11">
+      <x:c r="A5" s="2" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D5" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H5" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I5" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J5" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K5" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:11">
+      <x:c r="A6" s="2" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B6" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C6" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E6" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F6" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H6" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I6" s="2" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="J6" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K6" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:11">
+      <x:c r="A7" s="2" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B7" s="2" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E7" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G7" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H7" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I7" s="2" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="J7" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K7" s="2" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:11">
+      <x:c r="A8" s="2" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B8" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C8" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G8" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H8" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I8" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J8" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K8" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:11">
+      <x:c r="A9" s="2" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B9" s="2" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="C9" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E9" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G9" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H9" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I9" s="2" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="J9" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K9" s="2" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:11">
+      <x:c r="A10" s="2" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B10" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C10" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D10" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E10" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H10" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I10" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J10" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="K10" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:11">
+      <x:c r="A11" s="2" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B11" s="2" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C11" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E11" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="F11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G11" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H11" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I11" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J11" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K11" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:11">
+      <x:c r="A12" s="2" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B12" s="2" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C12" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F12" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H12" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I12" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J12" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="K12" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:11">
+      <x:c r="A13" s="2" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B13" s="2" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C13" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H13" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I13" s="2" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="J13" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="K13" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:11">
+      <x:c r="A14" s="2" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B14" s="2" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C14" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F14" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H14" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I14" s="2" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="J14" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="K14" s="2" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:11">
+      <x:c r="A15" s="2" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B15" s="2" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C15" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F15" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G15" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H15" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I15" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="J15" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="K15" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:11">
+      <x:c r="A16" s="2" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B16" s="2" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C16" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D16" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H16" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I16" s="2" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="J16" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="K16" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:11">
+      <x:c r="A17" s="2" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B17" s="2" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C17" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E17" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="G17" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H17" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="I17" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="J17" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="K17" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:sheetPr>

</xml_diff>